<commit_message>
Correct table 2 data
</commit_message>
<xml_diff>
--- a/Figures_Tables/Table2.xlsx
+++ b/Figures_Tables/Table2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">Disease</t>
   </si>
@@ -65,10 +65,13 @@
     <t xml:space="preserve">2005-2017</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00</t>
+    <t xml:space="preserve">13.38</t>
   </si>
   <si>
     <t xml:space="preserve">2018-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.60</t>
   </si>
   <si>
     <t xml:space="preserve">Varicella</t>
@@ -492,41 +495,41 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>